<commit_message>
iniciando calculo do consumo de um prato
</commit_message>
<xml_diff>
--- a/spreadsheets/GP.xlsx
+++ b/spreadsheets/GP.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="36">
   <si>
     <t>Arroz</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Matéria Prima</t>
+  </si>
+  <si>
+    <t>Mínimo</t>
   </si>
 </sst>
 </file>
@@ -213,7 +216,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,6 +250,10 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -562,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03EFE0A-A56E-4869-BBD8-BCA6F46ADE19}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -575,15 +582,14 @@
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>34</v>
       </c>
@@ -599,26 +605,29 @@
       <c r="E1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
@@ -635,26 +644,30 @@
         <f t="shared" ref="E2:E13" si="0">C2*D2</f>
         <v>3848</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2">
+        <f>C2/2</f>
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="K2" s="1">
         <v>25</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>2</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -671,27 +684,31 @@
         <f t="shared" si="0"/>
         <v>1440</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3">
+        <f t="shared" ref="F3:F13" si="1">C3/2</f>
+        <v>180</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>3</v>
       </c>
-      <c r="J3" s="1">
-        <f>I3*100</f>
+      <c r="K3" s="1">
+        <f>J3*100</f>
         <v>300</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>2</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -708,8 +725,12 @@
         <f t="shared" si="0"/>
         <v>1680</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>5</v>
       </c>
@@ -726,8 +747,12 @@
         <f t="shared" si="0"/>
         <v>19.200000000000003</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>8</v>
       </c>
@@ -744,8 +769,12 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>9</v>
       </c>
@@ -762,8 +791,12 @@
         <f t="shared" si="0"/>
         <v>14.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>10</v>
       </c>
@@ -780,8 +813,12 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>11</v>
       </c>
@@ -798,8 +835,12 @@
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>12</v>
       </c>
@@ -816,8 +857,12 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>13</v>
       </c>
@@ -834,8 +879,12 @@
         <f t="shared" si="0"/>
         <v>2160</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
@@ -852,8 +901,13 @@
         <f t="shared" si="0"/>
         <v>360</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>15</v>
       </c>
@@ -870,9 +924,14 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -881,7 +940,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>